<commit_message>
upated the date componet and plots
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Desktop\Final-Research-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D7EB48-3544-45D9-826D-6BBB306E4476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D35158-44E3-462F-8232-47412FF8F78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7785" activeTab="2" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="86">
   <si>
     <t xml:space="preserve"> Financial Year</t>
   </si>
@@ -302,8 +303,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -350,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -358,12 +360,35 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 5" xfId="1" xr:uid="{217EDFFB-1B0A-47F0-86B6-022F845F20DE}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6669,16 +6694,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>80961</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6706,15 +6731,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6741,16 +6766,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>166686</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>100011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>752474</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447674</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6778,15 +6803,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7113,8 +7138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86548ECB-474C-4C82-AFCD-DCE8D6396C69}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8770,7 +8795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8508772-BEF4-4C79-A19E-591393B8EA5B}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="F57" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M62"/>
     </sheetView>
   </sheetViews>
@@ -11743,20 +11768,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750171C9-C24E-4302-9158-F16F3E39D7C7}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:G62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -11779,8 +11807,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
+      <c r="A2" s="8">
+        <v>22098</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -11789,21 +11817,22 @@
         <v>42.30083857442348</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>E2</f>
+        <v>19.768089800000002</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>19.768089800000002</v>
       </c>
       <c r="F2">
-        <v>-42.30083857442348</v>
+        <v>-42.300838574423501</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>69.06119799999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>8</v>
+      <c r="A3" s="8">
+        <v>22463</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -11812,21 +11841,22 @@
         <v>44.152410901467505</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <f t="shared" ref="D3:D10" si="0">E3</f>
+        <v>5.2824671999999993</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>5.2824671999999993</v>
       </c>
       <c r="F3">
         <v>-44.152410901467505</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>17.147871999999992</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
+      <c r="A4" s="8">
+        <v>22828</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -11835,21 +11865,22 @@
         <v>44.901257861635223</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-4.3430757999999869</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-4.3430757999999869</v>
       </c>
       <c r="F4">
         <v>-44.901257861635223</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-35.039658000000017</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
+      <c r="A5" s="8">
+        <v>23193</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -11858,21 +11889,22 @@
         <v>51.614779874213838</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-9.9870591999999974</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-9.9870591999999974</v>
       </c>
       <c r="F5">
         <v>-51.614779874213838</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>-88.144592000000003</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
+      <c r="A6" s="8">
+        <v>23559</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -11881,21 +11913,22 @@
         <v>58.905660377358494</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-12.445875000000008</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-12.445875000000008</v>
       </c>
       <c r="F6">
         <v>-58.905660377358494</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>-143.01124999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
+      <c r="A7" s="8">
+        <v>23924</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -11904,21 +11937,22 @@
         <v>88.487394957983184</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-12.43549119999998</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>-12.43549119999998</v>
       </c>
       <c r="F7">
         <v>-88.487394957983184</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>-200.65411200000005</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
+      <c r="A8" s="8">
+        <v>24289</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -11927,21 +11961,22 @@
         <v>92.577030812324921</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-10.593299799999976</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-10.593299799999976</v>
       </c>
       <c r="F8">
         <v>-62.337635630468554</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>-262.228298</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
+      <c r="A9" s="8">
+        <v>24654</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -11950,21 +11985,22 @@
         <v>96.764705882352942</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-7.4801088000000036</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-7.4801088000000036</v>
       </c>
       <c r="F9">
         <v>-59.566751278643714</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>-329.00148799999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
+      <c r="A10" s="8">
+        <v>25020</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -11973,21 +12009,22 @@
         <v>103.78151260504201</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>-3.5822782000000117</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-3.5822782000000117</v>
       </c>
       <c r="F10">
         <v>-55.006727549518878</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>-402.32728199999997</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
+      <c r="A11" s="8">
+        <v>25385</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -11996,21 +12033,22 @@
         <v>116.90476190476188</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <f>E11</f>
+        <v>0.68600000000001415</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.68600000000001415</v>
       </c>
       <c r="F11">
         <v>-56.997354712814328</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>-483.62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>17</v>
+      <c r="A12" s="8">
+        <v>25750</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -12028,12 +12066,12 @@
         <v>-61.257605442055009</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>-574.33092199999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
+      <c r="A13" s="8">
+        <v>26115</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -12051,12 +12089,12 @@
         <v>-122.62218651284857</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>-675.92596800000013</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
+      <c r="A14" s="8">
+        <v>26481</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -12074,12 +12112,12 @@
         <v>-128.70141802759881</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>-789.86481800000013</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
+      <c r="A15" s="8">
+        <v>26846</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -12097,12 +12135,12 @@
         <v>-157.04574033071117</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>-917.58147199999996</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
+      <c r="A16" s="8">
+        <v>27211</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -12120,12 +12158,12 @@
         <v>-205.42956371259169</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>-1060.4662500000002</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
+      <c r="A17" s="8">
+        <v>27576</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -12143,12 +12181,12 @@
         <v>-225.97333206044573</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>-1219.8492320000003</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>23</v>
+      <c r="A18" s="8">
+        <v>27942</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -12166,12 +12204,12 @@
         <v>-231.45913140663848</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>-1396.9851380000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>24</v>
+      <c r="A19" s="8">
+        <v>28307</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -12189,12 +12227,12 @@
         <v>-272.99794832058399</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>-1593.0396480000002</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>25</v>
+      <c r="A20" s="8">
+        <v>28672</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -12212,12 +12250,12 @@
         <v>-208.34709112157037</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>-1809.0771620000003</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>26</v>
+      <c r="A21" s="8">
+        <v>29037</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -12235,12 +12273,12 @@
         <v>-196.61647884443153</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>-2046.05</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>27</v>
+      <c r="A22" s="8">
+        <v>29403</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -12258,12 +12296,12 @@
         <v>-37.324276848304081</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>-2304.7890419999999</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>28</v>
+      <c r="A23" s="8">
+        <v>29768</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -12272,10 +12310,11 @@
         <v>133.72999999999999</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <f>E23</f>
+        <v>16.802499200000149</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>16.802499200000149</v>
       </c>
       <c r="F23">
         <v>208.58830259454444</v>
@@ -12285,8 +12324,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>29</v>
+      <c r="A24" s="8">
+        <v>30133</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -12308,8 +12347,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
+      <c r="A25" s="8">
+        <v>30498</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -12318,10 +12357,11 @@
         <v>224.03333333333336</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <f>E25</f>
+        <v>15.709164800000032</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>15.709164800000032</v>
       </c>
       <c r="F25">
         <v>173.51649716174347</v>
@@ -12331,8 +12371,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>31</v>
+      <c r="A26" s="8">
+        <v>30864</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -12341,10 +12381,11 @@
         <v>361.56474770543372</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <f>E26</f>
+        <v>16.254125000000023</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>16.254125000000023</v>
       </c>
       <c r="F26">
         <v>12.92539543393076</v>
@@ -12354,8 +12395,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>32</v>
+      <c r="A27" s="8">
+        <v>31229</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -12377,8 +12418,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>33</v>
+      <c r="A28" s="8">
+        <v>31594</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -12387,10 +12428,11 @@
         <v>392.32321221278397</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <f>E28</f>
+        <v>21.087132199999679</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>21.087132199999679</v>
       </c>
       <c r="F28">
         <v>-179.13169343278398</v>
@@ -12400,8 +12442,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>34</v>
+      <c r="A29" s="8">
+        <v>31959</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -12410,10 +12452,11 @@
         <v>626.95116146623457</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <f>E29</f>
+        <v>26.030259200000366</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>26.030259200000366</v>
       </c>
       <c r="F29">
         <v>-626.95116146623457</v>
@@ -12423,8 +12466,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>35</v>
+      <c r="A30" s="8">
+        <v>32325</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -12446,8 +12489,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>36</v>
+      <c r="A31" s="8">
+        <v>32690</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -12469,8 +12512,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>37</v>
+      <c r="A32" s="8">
+        <v>33055</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -12492,8 +12535,8 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>38</v>
+      <c r="A33" s="8">
+        <v>33420</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -12515,8 +12558,8 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>39</v>
+      <c r="A34" s="8">
+        <v>33786</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -12538,8 +12581,8 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>40</v>
+      <c r="A35" s="8">
+        <v>34151</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -12561,8 +12604,8 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>41</v>
+      <c r="A36" s="8">
+        <v>34516</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -12584,8 +12627,8 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>42</v>
+      <c r="A37" s="8">
+        <v>34881</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -12607,8 +12650,8 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>43</v>
+      <c r="A38" s="8">
+        <v>35247</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -12630,8 +12673,8 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>44</v>
+      <c r="A39" s="8">
+        <v>35612</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -12653,8 +12696,8 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>45</v>
+      <c r="A40" s="8">
+        <v>35977</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -12676,8 +12719,8 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>46</v>
+      <c r="A41" s="8">
+        <v>36342</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -12699,8 +12742,8 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>47</v>
+      <c r="A42" s="8">
+        <v>36708</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -12722,8 +12765,8 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>48</v>
+      <c r="A43" s="8">
+        <v>37073</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -12745,8 +12788,8 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>49</v>
+      <c r="A44" s="8">
+        <v>37438</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -12768,8 +12811,8 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>50</v>
+      <c r="A45" s="8">
+        <v>37803</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -12791,8 +12834,8 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>51</v>
+      <c r="A46" s="8">
+        <v>38169</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -12814,8 +12857,8 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>52</v>
+      <c r="A47" s="8">
+        <v>38534</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -12837,8 +12880,8 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>53</v>
+      <c r="A48" s="8">
+        <v>38899</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -12860,8 +12903,8 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>54</v>
+      <c r="A49" s="8">
+        <v>39264</v>
       </c>
       <c r="B49">
         <v>48</v>
@@ -12883,8 +12926,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>55</v>
+      <c r="A50" s="8">
+        <v>39630</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -12906,8 +12949,8 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>56</v>
+      <c r="A51" s="8">
+        <v>39995</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -12929,8 +12972,8 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>57</v>
+      <c r="A52" s="8">
+        <v>40360</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -12952,8 +12995,8 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>58</v>
+      <c r="A53" s="8">
+        <v>40725</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -12975,8 +13018,8 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>59</v>
+      <c r="A54" s="8">
+        <v>41091</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -12998,8 +13041,8 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>60</v>
+      <c r="A55" s="8">
+        <v>41456</v>
       </c>
       <c r="B55">
         <v>54</v>
@@ -13021,8 +13064,8 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>61</v>
+      <c r="A56" s="8">
+        <v>41821</v>
       </c>
       <c r="B56">
         <v>55</v>
@@ -13044,8 +13087,8 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>62</v>
+      <c r="A57" s="8">
+        <v>42186</v>
       </c>
       <c r="B57">
         <v>56</v>
@@ -13067,8 +13110,8 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>63</v>
+      <c r="A58" s="8">
+        <v>42552</v>
       </c>
       <c r="B58">
         <v>57</v>
@@ -13090,8 +13133,8 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>64</v>
+      <c r="A59" s="8">
+        <v>42917</v>
       </c>
       <c r="B59">
         <v>58</v>
@@ -13113,8 +13156,8 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>65</v>
+      <c r="A60" s="8">
+        <v>43282</v>
       </c>
       <c r="B60">
         <v>59</v>
@@ -13136,8 +13179,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>66</v>
+      <c r="A61" s="8">
+        <v>43647</v>
       </c>
       <c r="B61">
         <v>60</v>
@@ -13159,8 +13202,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>67</v>
+      <c r="A62" s="8">
+        <v>44013</v>
       </c>
       <c r="B62">
         <v>61</v>
@@ -13182,26 +13225,1514 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63">
-        <v>62</v>
-      </c>
-      <c r="C63">
-        <v>4043.4701516952782</v>
-      </c>
+      <c r="A63" s="8"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A63">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=" Financial Year">
+    <cfRule type="uniqueValues" dxfId="3" priority="1"/>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text=" Financial Year">
       <formula>NOT(ISERROR(SEARCH(" Financial Year",A1)))</formula>
     </cfRule>
-    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:A63" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2F29B6-EF92-4EE0-A82D-A0FA9527810B}">
+  <dimension ref="A1:I62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>22098</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>42.30083857442348</v>
+      </c>
+      <c r="D2">
+        <v>19.768089799999998</v>
+      </c>
+      <c r="E2">
+        <v>19.768089799999998</v>
+      </c>
+      <c r="F2">
+        <v>42.300838574423501</v>
+      </c>
+      <c r="G2">
+        <v>69.06119799999999</v>
+      </c>
+      <c r="I2">
+        <f>ABS(D2)</f>
+        <v>19.768089799999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>22463</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>44.152410901467505</v>
+      </c>
+      <c r="D3">
+        <v>5.2824671999999993</v>
+      </c>
+      <c r="E3">
+        <v>5.2824671999999993</v>
+      </c>
+      <c r="F3">
+        <v>44.152410901467505</v>
+      </c>
+      <c r="G3">
+        <v>17.147871999999992</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="0">ABS(D3)</f>
+        <v>5.2824671999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>22828</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>44.901257861635223</v>
+      </c>
+      <c r="D4">
+        <v>4.3430757999999869</v>
+      </c>
+      <c r="E4">
+        <v>4.3430757999999869</v>
+      </c>
+      <c r="F4">
+        <v>44.901257861635223</v>
+      </c>
+      <c r="G4">
+        <v>35.039658000000017</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>4.3430757999999869</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>23193</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>51.614779874213838</v>
+      </c>
+      <c r="D5">
+        <v>9.9870591999999974</v>
+      </c>
+      <c r="E5">
+        <v>9.9870591999999974</v>
+      </c>
+      <c r="F5">
+        <v>51.614779874213838</v>
+      </c>
+      <c r="G5">
+        <v>88.144592000000003</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>9.9870591999999974</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>23559</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>58.905660377358494</v>
+      </c>
+      <c r="D6">
+        <v>12.445875000000008</v>
+      </c>
+      <c r="E6">
+        <v>12.445875000000008</v>
+      </c>
+      <c r="F6">
+        <v>58.905660377358494</v>
+      </c>
+      <c r="G6">
+        <v>143.01124999999996</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>12.445875000000008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>23924</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>88.487394957983184</v>
+      </c>
+      <c r="D7">
+        <v>12.43549119999998</v>
+      </c>
+      <c r="E7">
+        <v>12.43549119999998</v>
+      </c>
+      <c r="F7">
+        <v>88.487394957983184</v>
+      </c>
+      <c r="G7">
+        <v>200.65411200000005</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>12.43549119999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>24289</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>92.577030812324921</v>
+      </c>
+      <c r="D8">
+        <v>10.593299799999976</v>
+      </c>
+      <c r="E8">
+        <v>10.593299799999976</v>
+      </c>
+      <c r="F8">
+        <v>62.337635630468554</v>
+      </c>
+      <c r="G8">
+        <v>262.228298</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>10.593299799999976</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>24654</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>96.764705882352942</v>
+      </c>
+      <c r="D9">
+        <v>7.4801088000000036</v>
+      </c>
+      <c r="E9">
+        <v>7.4801088000000036</v>
+      </c>
+      <c r="F9">
+        <v>59.566751278643714</v>
+      </c>
+      <c r="G9">
+        <v>329.00148799999999</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>7.4801088000000036</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>25020</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>103.78151260504201</v>
+      </c>
+      <c r="D10">
+        <v>3.5822782000000117</v>
+      </c>
+      <c r="E10">
+        <v>3.5822782000000117</v>
+      </c>
+      <c r="F10">
+        <v>55.006727549518878</v>
+      </c>
+      <c r="G10">
+        <v>402.32728199999997</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>3.5822782000000117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>25385</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>116.90476190476188</v>
+      </c>
+      <c r="D11">
+        <f>E11</f>
+        <v>0.68600000000001415</v>
+      </c>
+      <c r="E11">
+        <v>0.68600000000001415</v>
+      </c>
+      <c r="F11">
+        <v>56.997354712814328</v>
+      </c>
+      <c r="G11">
+        <v>483.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>25750</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>126.00840336134453</v>
+      </c>
+      <c r="D12">
+        <v>4.2</v>
+      </c>
+      <c r="E12">
+        <v>4.2</v>
+      </c>
+      <c r="F12">
+        <v>61.257605442055009</v>
+      </c>
+      <c r="G12">
+        <v>574.33092199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>26115</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>141.77871148459383</v>
+      </c>
+      <c r="D13">
+        <v>1.2</v>
+      </c>
+      <c r="E13">
+        <v>1.2</v>
+      </c>
+      <c r="F13">
+        <v>122.62218651284857</v>
+      </c>
+      <c r="G13">
+        <v>675.92596800000013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>26481</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>149.15966386554621</v>
+      </c>
+      <c r="D14">
+        <v>11.9</v>
+      </c>
+      <c r="E14">
+        <v>11.9</v>
+      </c>
+      <c r="F14">
+        <v>128.70141802759881</v>
+      </c>
+      <c r="G14">
+        <v>789.86481800000013</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>26846</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>170.25210084033614</v>
+      </c>
+      <c r="D15">
+        <v>5.2</v>
+      </c>
+      <c r="E15">
+        <v>5.2</v>
+      </c>
+      <c r="F15">
+        <v>157.04574033071117</v>
+      </c>
+      <c r="G15">
+        <v>917.58147199999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>27211</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>210.01426533523539</v>
+      </c>
+      <c r="D16">
+        <v>1.7</v>
+      </c>
+      <c r="E16">
+        <v>1.7</v>
+      </c>
+      <c r="F16">
+        <v>205.42956371259169</v>
+      </c>
+      <c r="G16">
+        <v>1060.4662500000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>27576</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>235.95555555555558</v>
+      </c>
+      <c r="D17">
+        <v>2.1</v>
+      </c>
+      <c r="E17">
+        <v>2.1</v>
+      </c>
+      <c r="F17">
+        <v>225.97333206044573</v>
+      </c>
+      <c r="G17">
+        <v>1219.8492320000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>27942</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>244.73</v>
+      </c>
+      <c r="D18">
+        <v>2.0499999</v>
+      </c>
+      <c r="E18">
+        <v>2.0499999</v>
+      </c>
+      <c r="F18">
+        <v>231.45913140663848</v>
+      </c>
+      <c r="G18">
+        <v>1396.9851380000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>28307</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>293.64705882352939</v>
+      </c>
+      <c r="D19">
+        <v>0.8</v>
+      </c>
+      <c r="E19">
+        <v>0.8</v>
+      </c>
+      <c r="F19">
+        <v>272.99794832058399</v>
+      </c>
+      <c r="G19">
+        <v>1593.0396480000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>28672</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>242.02608695652174</v>
+      </c>
+      <c r="D20">
+        <v>1.97</v>
+      </c>
+      <c r="E20">
+        <v>1.97</v>
+      </c>
+      <c r="F20">
+        <v>208.34709112157037</v>
+      </c>
+      <c r="G20">
+        <v>1809.0771620000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>29037</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>213.9025</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>196.61647884443153</v>
+      </c>
+      <c r="G21">
+        <v>2046.05</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>29403</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>124.461</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>37.324276848304081</v>
+      </c>
+      <c r="G22">
+        <v>2304.7890419999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>29768</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>133.72999999999999</v>
+      </c>
+      <c r="D23">
+        <f>E23</f>
+        <v>16.802499200000149</v>
+      </c>
+      <c r="E23">
+        <v>16.802499200000149</v>
+      </c>
+      <c r="F23">
+        <v>208.58830259454444</v>
+      </c>
+      <c r="G23">
+        <v>1565.2162708415501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>30133</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>217.75</v>
+      </c>
+      <c r="D24">
+        <v>2.02</v>
+      </c>
+      <c r="E24">
+        <v>2.02</v>
+      </c>
+      <c r="F24">
+        <v>46.154135107221691</v>
+      </c>
+      <c r="G24">
+        <v>543.26640510304696</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>30498</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>224.03333333333336</v>
+      </c>
+      <c r="D25">
+        <f>E25</f>
+        <v>15.709164800000032</v>
+      </c>
+      <c r="E25">
+        <v>15.709164800000032</v>
+      </c>
+      <c r="F25">
+        <v>173.51649716174347</v>
+      </c>
+      <c r="G25">
+        <v>429.77464486072699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>30864</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>361.56474770543372</v>
+      </c>
+      <c r="D26">
+        <f>E26</f>
+        <v>16.254125000000023</v>
+      </c>
+      <c r="E26">
+        <v>16.254125000000023</v>
+      </c>
+      <c r="F26">
+        <v>12.92539543393076</v>
+      </c>
+      <c r="G26">
+        <v>293.63133617189402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>31229</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>351.96663385245415</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>216.27077542096731</v>
+      </c>
+      <c r="G27">
+        <v>384.63216488538097</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>31594</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>392.32321221278397</v>
+      </c>
+      <c r="D28">
+        <f>E28</f>
+        <v>21.087132199999679</v>
+      </c>
+      <c r="E28">
+        <v>21.087132199999679</v>
+      </c>
+      <c r="F28">
+        <v>179.13169343278398</v>
+      </c>
+      <c r="G28">
+        <v>401.52703667273499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>31959</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>626.95116146623457</v>
+      </c>
+      <c r="D29">
+        <f>E29</f>
+        <v>26.030259200000366</v>
+      </c>
+      <c r="E29">
+        <v>26.030259200000366</v>
+      </c>
+      <c r="F29">
+        <v>626.95116146623457</v>
+      </c>
+      <c r="G29">
+        <v>511.28822370242102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>32325</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>650.89316516666668</v>
+      </c>
+      <c r="D30">
+        <v>4.7</v>
+      </c>
+      <c r="E30">
+        <v>4.7</v>
+      </c>
+      <c r="F30">
+        <v>650.89316516666668</v>
+      </c>
+      <c r="G30">
+        <v>470.09228354012299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>32690</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>527.64809859993659</v>
+      </c>
+      <c r="D31">
+        <v>1.76</v>
+      </c>
+      <c r="E31">
+        <v>1.76</v>
+      </c>
+      <c r="F31">
+        <v>527.64809859993659</v>
+      </c>
+      <c r="G31">
+        <v>384.99517293613701</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>33055</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>430.439886588268</v>
+      </c>
+      <c r="D32">
+        <v>5.91</v>
+      </c>
+      <c r="E32">
+        <v>5.91</v>
+      </c>
+      <c r="F32">
+        <v>430.439886588268</v>
+      </c>
+      <c r="G32">
+        <v>244.39075838208399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>33420</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>332.17290571221542</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>332.17290571221542</v>
+      </c>
+      <c r="G33">
+        <v>179.474769912619</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>33786</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>285.74578600508755</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>71.390964379176268</v>
+      </c>
+      <c r="G34">
+        <v>120.252259985827</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>34151</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>322.04390441894867</v>
+      </c>
+      <c r="D35">
+        <v>54.6</v>
+      </c>
+      <c r="E35">
+        <v>54.6</v>
+      </c>
+      <c r="F35">
+        <v>234.62134982143192</v>
+      </c>
+      <c r="G35">
+        <v>118.786060581379</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>34516</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>399.04304467121597</v>
+      </c>
+      <c r="D36">
+        <v>88.2</v>
+      </c>
+      <c r="E36">
+        <v>88.2</v>
+      </c>
+      <c r="F36">
+        <v>333.74990899275576</v>
+      </c>
+      <c r="G36">
+        <v>148.49891681729699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>34881</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>575.58189474212497</v>
+      </c>
+      <c r="D37">
+        <v>121.2</v>
+      </c>
+      <c r="E37">
+        <v>121.2</v>
+      </c>
+      <c r="F37">
+        <v>393.25689135142682</v>
+      </c>
+      <c r="G37">
+        <v>145.151216117594</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>35247</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>604.45853269380007</v>
+      </c>
+      <c r="D38">
+        <v>121</v>
+      </c>
+      <c r="E38">
+        <v>121</v>
+      </c>
+      <c r="F38">
+        <v>363.24556083330401</v>
+      </c>
+      <c r="G38">
+        <v>145.534630500829</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>35612</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>626.93333131710835</v>
+      </c>
+      <c r="D39">
+        <v>175</v>
+      </c>
+      <c r="E39">
+        <v>175</v>
+      </c>
+      <c r="F39">
+        <v>265.30839155189</v>
+      </c>
+      <c r="G39">
+        <v>152.516808731092</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>35977</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>658.48158465275378</v>
+      </c>
+      <c r="D40">
+        <v>210</v>
+      </c>
+      <c r="E40">
+        <v>210</v>
+      </c>
+      <c r="F40">
+        <v>130.64011205405677</v>
+      </c>
+      <c r="G40">
+        <v>135.617944882106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>36342</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>599.85632579465891</v>
+      </c>
+      <c r="D41">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="E41">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="F41">
+        <v>56.713906355499148</v>
+      </c>
+      <c r="G41">
+        <v>123.43242395845</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>36708</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>619.32468370968729</v>
+      </c>
+      <c r="D42">
+        <v>160.69999999999999</v>
+      </c>
+      <c r="E42">
+        <v>160.69999999999999</v>
+      </c>
+      <c r="F42">
+        <v>108.34913323242097</v>
+      </c>
+      <c r="G42">
+        <v>117.002584885845</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>37073</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>584.05038685724548</v>
+      </c>
+      <c r="D43">
+        <v>151.496150651927</v>
+      </c>
+      <c r="E43">
+        <v>151.496150651927</v>
+      </c>
+      <c r="F43">
+        <v>235.94725715903053</v>
+      </c>
+      <c r="G43">
+        <v>114.128259060837</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>37438</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>617.85635908925371</v>
+      </c>
+      <c r="D44">
+        <v>184.6480591975</v>
+      </c>
+      <c r="E44">
+        <v>184.6480591975</v>
+      </c>
+      <c r="F44">
+        <v>201.17006801667731</v>
+      </c>
+      <c r="G44">
+        <v>109.21191184217101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>37803</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>660.68843907801886</v>
+      </c>
+      <c r="D45">
+        <v>202.19259361849998</v>
+      </c>
+      <c r="E45">
+        <v>202.19259361849998</v>
+      </c>
+      <c r="F45">
+        <v>468.97337212392938</v>
+      </c>
+      <c r="G45">
+        <v>95.845581597459301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>38169</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>793.94874738631825</v>
+      </c>
+      <c r="D46">
+        <v>295.416479800692</v>
+      </c>
+      <c r="E46">
+        <v>295.416479800692</v>
+      </c>
+      <c r="F46">
+        <v>592.7103272756101</v>
+      </c>
+      <c r="G46">
+        <v>99.447858634069306</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>38534</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>923.92218585583873</v>
+      </c>
+      <c r="D47">
+        <v>379.80834066706097</v>
+      </c>
+      <c r="E47">
+        <v>379.80834066706097</v>
+      </c>
+      <c r="F47">
+        <v>580.91762229240112</v>
+      </c>
+      <c r="G47">
+        <v>104.161592504748</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>38899</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>997.76476446995264</v>
+      </c>
+      <c r="D48">
+        <v>644.26249994651198</v>
+      </c>
+      <c r="E48">
+        <v>644.26249994651198</v>
+      </c>
+      <c r="F48">
+        <v>1068.897791475551</v>
+      </c>
+      <c r="G48">
+        <v>104.377585567366</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>39264</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>1190.2564401323843</v>
+      </c>
+      <c r="D49">
+        <v>792.30578089124401</v>
+      </c>
+      <c r="E49">
+        <v>792.30578089124401</v>
+      </c>
+      <c r="F49">
+        <v>1677.4219135928251</v>
+      </c>
+      <c r="G49">
+        <v>107.96589537320899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>39630</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>1444.0404021488146</v>
+      </c>
+      <c r="D50">
+        <v>728.86090065240796</v>
+      </c>
+      <c r="E50">
+        <v>728.86090065240796</v>
+      </c>
+      <c r="F50">
+        <v>1470.5614459428223</v>
+      </c>
+      <c r="G50">
+        <v>111.311992506636</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>39995</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>2512.7805566451116</v>
+      </c>
+      <c r="D51">
+        <v>841.57080274763598</v>
+      </c>
+      <c r="E51">
+        <v>812.72032169957606</v>
+      </c>
+      <c r="F51">
+        <v>56.111982776657442</v>
+      </c>
+      <c r="G51">
+        <v>108.319176300047</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>40360</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>2667.3441667281536</v>
+      </c>
+      <c r="D52">
+        <v>543.87272727272796</v>
+      </c>
+      <c r="E52">
+        <v>506.65842345964001</v>
+      </c>
+      <c r="F52">
+        <v>166.70339234882567</v>
+      </c>
+      <c r="G52">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>40725</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>2787.1725205571438</v>
+      </c>
+      <c r="D53">
+        <v>894.293858</v>
+      </c>
+      <c r="E53">
+        <v>906.14042758727601</v>
+      </c>
+      <c r="F53">
+        <v>285.0118475571976</v>
+      </c>
+      <c r="G53">
+        <v>93.066503735108299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>41091</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>2730.5915761291758</v>
+      </c>
+      <c r="D54">
+        <v>1205.3884877937401</v>
+      </c>
+      <c r="E54">
+        <v>1159.0514597205299</v>
+      </c>
+      <c r="F54">
+        <v>645.02714536483609</v>
+      </c>
+      <c r="G54">
+        <v>103.581529116697</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>41456</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>2891.5786996551833</v>
+      </c>
+      <c r="D55">
+        <v>1096</v>
+      </c>
+      <c r="E55">
+        <v>1051.62292249344</v>
+      </c>
+      <c r="F55">
+        <v>398.08720973481604</v>
+      </c>
+      <c r="G55">
+        <v>104.487341700489</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>41821</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>3261.2397758457892</v>
+      </c>
+      <c r="D56">
+        <v>1058.56454034685</v>
+      </c>
+      <c r="E56">
+        <v>1031.54624299492</v>
+      </c>
+      <c r="F56">
+        <v>56.925398460893121</v>
+      </c>
+      <c r="G56">
+        <v>106.106235195211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>42186</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>3238.7183844669862</v>
+      </c>
+      <c r="D57">
+        <v>737.65214015142794</v>
+      </c>
+      <c r="E57">
+        <v>737.36952105303396</v>
+      </c>
+      <c r="F57">
+        <v>74.069725709489376</v>
+      </c>
+      <c r="G57">
+        <v>100.98705396656</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>42552</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>2920.3988814897266</v>
+      </c>
+      <c r="D58">
+        <v>625.70436186706809</v>
+      </c>
+      <c r="E58">
+        <v>625.55896416211999</v>
+      </c>
+      <c r="F58">
+        <v>622.06287846039913</v>
+      </c>
+      <c r="G58">
+        <v>96.130690827214494</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>42917</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <v>3074.4473911531209</v>
+      </c>
+      <c r="D59">
+        <v>802.70414100856806</v>
+      </c>
+      <c r="E59">
+        <v>802.40000875549993</v>
+      </c>
+      <c r="F59">
+        <v>754.03964403867303</v>
+      </c>
+      <c r="G59">
+        <v>93.678152818193894</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>43282</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>3292.7025573429642</v>
+      </c>
+      <c r="D60">
+        <v>1055.3533526303299</v>
+      </c>
+      <c r="E60">
+        <v>1055.03170652842</v>
+      </c>
+      <c r="F60">
+        <v>447.56604216772257</v>
+      </c>
+      <c r="G60">
+        <v>90.086175339845695</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>43647</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <v>3535.306063420217</v>
+      </c>
+      <c r="D61">
+        <v>1273.8855862508599</v>
+      </c>
+      <c r="E61">
+        <v>1273.5599490392899</v>
+      </c>
+      <c r="F61">
+        <v>264.76882550326991</v>
+      </c>
+      <c r="G61">
+        <v>93.296236571518506</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>44013</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <v>3760.036818093995</v>
+      </c>
+      <c r="D62">
+        <v>873.79283455531709</v>
+      </c>
+      <c r="E62">
+        <v>873.46822523084199</v>
+      </c>
+      <c r="F62">
+        <v>544.73543406991757</v>
+      </c>
+      <c r="G62">
+        <v>94.995621691551804</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A62">
+    <cfRule type="uniqueValues" dxfId="1" priority="1"/>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text=" Financial Year">
+      <formula>NOT(ISERROR(SEARCH(" Financial Year",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new data to sheet 4
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Desktop\Final-Research-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A8D09-A11E-4587-AEF6-6A623B7FB5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75061872-132B-4F2C-AAD2-51CEDADD759C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
   <si>
     <t xml:space="preserve"> Financial Year</t>
   </si>
@@ -10189,8 +10189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8508772-BEF4-4C79-A19E-591393B8EA5B}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView topLeftCell="E39" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10636,7 +10636,7 @@
         <v>30.239395181856363</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K3:K62" si="7">L8/1000000</f>
+        <f t="shared" ref="K8:K62" si="7">L8/1000000</f>
         <v>30.239395181856363</v>
       </c>
       <c r="L8" s="5">
@@ -15068,8 +15068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2F29B6-EF92-4EE0-A82D-A0FA9527810B}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15081,6 +15081,7 @@
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -15105,6 +15106,9 @@
       <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
@@ -15128,6 +15132,9 @@
       <c r="G2">
         <v>69.06119799999999</v>
       </c>
+      <c r="H2">
+        <v>91.399000000000001</v>
+      </c>
       <c r="I2">
         <f>ABS(D2)</f>
         <v>19.768089799999998</v>
@@ -15155,6 +15162,9 @@
       <c r="G3">
         <v>17.147871999999992</v>
       </c>
+      <c r="H3">
+        <v>84.316000000000003</v>
+      </c>
       <c r="I3">
         <f t="shared" ref="I3:I10" si="0">ABS(D3)</f>
         <v>5.2824671999999993</v>
@@ -15182,6 +15192,9 @@
       <c r="G4">
         <v>35.039658000000017</v>
       </c>
+      <c r="H4">
+        <v>76.262</v>
+      </c>
       <c r="I4">
         <f t="shared" si="0"/>
         <v>4.3430757999999869</v>
@@ -15209,6 +15222,9 @@
       <c r="G5">
         <v>88.144592000000003</v>
       </c>
+      <c r="H5">
+        <v>67.432000000000002</v>
+      </c>
       <c r="I5">
         <f t="shared" si="0"/>
         <v>9.9870591999999974</v>
@@ -15236,6 +15252,9 @@
       <c r="G6">
         <v>143.01124999999996</v>
       </c>
+      <c r="H6">
+        <v>58.021000000000001</v>
+      </c>
       <c r="I6">
         <f t="shared" si="0"/>
         <v>12.445875000000008</v>
@@ -15263,6 +15282,9 @@
       <c r="G7">
         <v>200.65411200000005</v>
       </c>
+      <c r="H7">
+        <v>48.224000000000004</v>
+      </c>
       <c r="I7">
         <f t="shared" si="0"/>
         <v>12.43549119999998</v>
@@ -15290,6 +15312,9 @@
       <c r="G8">
         <v>262.228298</v>
       </c>
+      <c r="H8">
+        <v>30.239395181856363</v>
+      </c>
       <c r="I8">
         <f t="shared" si="0"/>
         <v>10.593299799999976</v>
@@ -15317,6 +15342,9 @@
       <c r="G9">
         <v>329.00148799999999</v>
       </c>
+      <c r="H9">
+        <v>37.197954603709228</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
         <v>7.4801088000000036</v>
@@ -15344,6 +15372,9 @@
       <c r="G10">
         <v>402.32728199999997</v>
       </c>
+      <c r="H10">
+        <v>48.774785055523132</v>
+      </c>
       <c r="I10">
         <f t="shared" si="0"/>
         <v>3.5822782000000117</v>
@@ -15372,6 +15403,9 @@
       <c r="G11">
         <v>483.62</v>
       </c>
+      <c r="H11">
+        <v>59.907407191947556</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -15395,6 +15429,9 @@
       <c r="G12">
         <v>574.33092199999999</v>
       </c>
+      <c r="H12">
+        <v>64.750797919289525</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -15418,6 +15455,9 @@
       <c r="G13">
         <v>675.92596800000013</v>
       </c>
+      <c r="H13">
+        <v>19.156524971745259</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
@@ -15441,6 +15481,9 @@
       <c r="G14">
         <v>789.86481800000013</v>
       </c>
+      <c r="H14">
+        <v>20.458245837947395</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -15464,6 +15507,9 @@
       <c r="G15">
         <v>917.58147199999996</v>
       </c>
+      <c r="H15">
+        <v>13.206360509624986</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
@@ -15487,8 +15533,11 @@
       <c r="G16">
         <v>1060.4662500000002</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>4.5847016226436983</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>27576</v>
       </c>
@@ -15510,8 +15559,11 @@
       <c r="G17">
         <v>1219.8492320000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>9.9822234951098423</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>27942</v>
       </c>
@@ -15533,8 +15585,11 @@
       <c r="G18">
         <v>1396.9851380000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>13.270868593361518</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>28307</v>
       </c>
@@ -15556,8 +15611,11 @@
       <c r="G19">
         <v>1593.0396480000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>20.649110502945412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>28672</v>
       </c>
@@ -15579,8 +15637,11 @@
       <c r="G20">
         <v>1809.0771620000003</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>33.67899583495138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>29037</v>
       </c>
@@ -15602,8 +15663,11 @@
       <c r="G21">
         <v>2046.05</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>17.286021155568488</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>29403</v>
       </c>
@@ -15625,8 +15689,11 @@
       <c r="G22">
         <v>2304.7890419999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>87.136723151695918</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>29768</v>
       </c>
@@ -15649,8 +15716,11 @@
       <c r="G23">
         <v>1565.2162708415501</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>342.31830259454443</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>30133</v>
       </c>
@@ -15672,8 +15742,11 @@
       <c r="G24">
         <v>543.26640510304696</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>263.90413510722169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>30498</v>
       </c>
@@ -15696,8 +15769,11 @@
       <c r="G25">
         <v>429.77464486072699</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>397.54983049507683</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>30864</v>
       </c>
@@ -15720,8 +15796,11 @@
       <c r="G26">
         <v>293.63133617189402</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>374.49014313936448</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>31229</v>
       </c>
@@ -15743,8 +15822,11 @@
       <c r="G27">
         <v>384.63216488538097</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>568.23740927342146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>31594</v>
       </c>
@@ -15767,8 +15849,11 @@
       <c r="G28">
         <v>401.52703667273499</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>213.19151878</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>31959</v>
       </c>
@@ -15791,8 +15876,11 @@
       <c r="G29">
         <v>511.28822370242102</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>32325</v>
       </c>
@@ -15814,8 +15902,11 @@
       <c r="G30">
         <v>470.09228354012299</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>32690</v>
       </c>
@@ -15837,8 +15928,11 @@
       <c r="G31">
         <v>384.99517293613701</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>33055</v>
       </c>
@@ -15860,8 +15954,11 @@
       <c r="G32">
         <v>244.39075838208399</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>33420</v>
       </c>
@@ -15883,8 +15980,11 @@
       <c r="G33">
         <v>179.474769912619</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>33786</v>
       </c>
@@ -15906,8 +16006,11 @@
       <c r="G34">
         <v>120.252259985827</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>214.35482162591128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>34151</v>
       </c>
@@ -15929,8 +16032,11 @@
       <c r="G35">
         <v>118.786060581379</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>87.422554597516736</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34516</v>
       </c>
@@ -15952,8 +16058,11 @@
       <c r="G36">
         <v>148.49891681729699</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>65.293135678460231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>34881</v>
       </c>
@@ -15975,8 +16084,11 @@
       <c r="G37">
         <v>145.151216117594</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>182.32500339069813</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>35247</v>
       </c>
@@ -15998,8 +16110,11 @@
       <c r="G38">
         <v>145.534630500829</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>241.21297186049603</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>35612</v>
       </c>
@@ -16021,8 +16136,11 @@
       <c r="G39">
         <v>152.516808731092</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>361.62493976521836</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>35977</v>
       </c>
@@ -16044,8 +16162,11 @@
       <c r="G40">
         <v>135.617944882106</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>527.84147259869701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>36342</v>
       </c>
@@ -16067,8 +16188,11 @@
       <c r="G41">
         <v>123.43242395845</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>543.14241943915977</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>36708</v>
       </c>
@@ -16090,8 +16214,11 @@
       <c r="G42">
         <v>117.002584885845</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>727.67381694210826</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>37073</v>
       </c>
@@ -16113,8 +16240,11 @@
       <c r="G43">
         <v>114.128259060837</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>819.99764401627601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>37438</v>
       </c>
@@ -16136,8 +16266,11 @@
       <c r="G44">
         <v>109.21191184217101</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>819.02642710593102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>37803</v>
       </c>
@@ -16159,8 +16292,11 @@
       <c r="G45">
         <v>95.845581597459301</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>1129.6618112019482</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>38169</v>
       </c>
@@ -16182,8 +16318,11 @@
       <c r="G46">
         <v>99.447858634069306</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>1386.6590746619283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>38534</v>
       </c>
@@ -16205,8 +16344,11 @@
       <c r="G47">
         <v>104.161592504748</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>1504.8398081482399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>38899</v>
       </c>
@@ -16228,8 +16370,11 @@
       <c r="G48">
         <v>104.377585567366</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>2066.6625559455038</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>39264</v>
       </c>
@@ -16251,8 +16396,11 @@
       <c r="G49">
         <v>107.96589537320899</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>2867.6783537252095</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>39630</v>
       </c>
@@ -16274,8 +16422,11 @@
       <c r="G50">
         <v>111.311992506636</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>2914.6018480916368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>39995</v>
       </c>
@@ -16297,8 +16448,11 @@
       <c r="G51">
         <v>108.319176300047</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>2568.892539421769</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>40360</v>
       </c>
@@ -16320,8 +16474,11 @@
       <c r="G52">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>2834.0475590769793</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>40725</v>
       </c>
@@ -16343,8 +16500,11 @@
       <c r="G53">
         <v>93.066503735108299</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>2502.1606729999462</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>41091</v>
       </c>
@@ -16366,8 +16526,11 @@
       <c r="G54">
         <v>103.581529116697</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>3375.6187214940119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>41456</v>
       </c>
@@ -16389,8 +16552,11 @@
       <c r="G55">
         <v>104.487341700489</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>3289.6659093899993</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>41821</v>
       </c>
@@ -16412,8 +16578,11 @@
       <c r="G56">
         <v>106.106235195211</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>3318.1651743066823</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>42186</v>
       </c>
@@ -16435,8 +16604,11 @@
       <c r="G57">
         <v>100.98705396656</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>3164.6486587574968</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>42552</v>
       </c>
@@ -16458,8 +16630,11 @@
       <c r="G58">
         <v>96.130690827214494</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>3542.4617599501257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>42917</v>
       </c>
@@ -16481,8 +16656,11 @@
       <c r="G59">
         <v>93.678152818193894</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>3828.4870351917939</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>43282</v>
       </c>
@@ -16504,8 +16682,11 @@
       <c r="G60">
         <v>90.086175339845695</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>3740.2685995106867</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>43647</v>
       </c>
@@ -16527,8 +16708,11 @@
       <c r="G61">
         <v>93.296236571518506</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>3800.0748889234869</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>44013</v>
       </c>
@@ -16549,6 +16733,9 @@
       </c>
       <c r="G62">
         <v>94.995621691551804</v>
+      </c>
+      <c r="H62">
+        <v>4304.7722521639125</v>
       </c>
     </row>
   </sheetData>
@@ -16559,5 +16746,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data shall on raw nfa makes it that u can predict
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Desktop\Final-Research-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75061872-132B-4F2C-AAD2-51CEDADD759C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC48B17-1279-46AB-ADD5-DC81EA4090EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
   </bookViews>
@@ -4904,7 +4904,7 @@
                   <c:v>58.021000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.224000000000004</c:v>
+                  <c:v>48.223999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30.239395181856363</c:v>
@@ -10189,8 +10189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8508772-BEF4-4C79-A19E-591393B8EA5B}">
   <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView topLeftCell="E39" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K62"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10579,7 +10579,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>48.224000000000004</v>
+        <v>48.223999999999997</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="5"/>
@@ -15066,10 +15066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2F29B6-EF92-4EE0-A82D-A0FA9527810B}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15084,7 +15084,7 @@
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>80</v>
       </c>
@@ -15110,7 +15110,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>22098</v>
       </c>
@@ -15135,12 +15135,8 @@
       <c r="H2">
         <v>91.399000000000001</v>
       </c>
-      <c r="I2">
-        <f>ABS(D2)</f>
-        <v>19.768089799999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>22463</v>
       </c>
@@ -15165,12 +15161,8 @@
       <c r="H3">
         <v>84.316000000000003</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I10" si="0">ABS(D3)</f>
-        <v>5.2824671999999993</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>22828</v>
       </c>
@@ -15195,12 +15187,8 @@
       <c r="H4">
         <v>76.262</v>
       </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>4.3430757999999869</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>23193</v>
       </c>
@@ -15225,12 +15213,8 @@
       <c r="H5">
         <v>67.432000000000002</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>9.9870591999999974</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>23559</v>
       </c>
@@ -15255,12 +15239,8 @@
       <c r="H6">
         <v>58.021000000000001</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>12.445875000000008</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>23924</v>
       </c>
@@ -15285,12 +15265,8 @@
       <c r="H7">
         <v>48.224000000000004</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>12.43549119999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>24289</v>
       </c>
@@ -15315,12 +15291,8 @@
       <c r="H8">
         <v>30.239395181856363</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>10.593299799999976</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>24654</v>
       </c>
@@ -15345,12 +15317,8 @@
       <c r="H9">
         <v>37.197954603709228</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>7.4801088000000036</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>25020</v>
       </c>
@@ -15375,12 +15343,8 @@
       <c r="H10">
         <v>48.774785055523132</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>3.5822782000000117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>25385</v>
       </c>
@@ -15407,7 +15371,7 @@
         <v>59.907407191947556</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>25750</v>
       </c>
@@ -15433,7 +15397,7 @@
         <v>64.750797919289525</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>26115</v>
       </c>
@@ -15459,7 +15423,7 @@
         <v>19.156524971745259</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>26481</v>
       </c>
@@ -15485,7 +15449,7 @@
         <v>20.458245837947395</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>26846</v>
       </c>
@@ -15511,7 +15475,7 @@
         <v>13.206360509624986</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>27211</v>
       </c>
@@ -15877,7 +15841,8 @@
         <v>511.28822370242102</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <f>0.0325*B2^3 - 0.6805*B2^2 - 5.269*B2 + 97.316</f>
+        <v>91.399000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -15903,7 +15868,8 @@
         <v>470.09228354012299</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <f t="shared" ref="H30:H33" si="0">0.0325*B3^3 - 0.6805*B3^2 - 5.269*B3 + 97.316</f>
+        <v>84.316000000000003</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -15929,7 +15895,8 @@
         <v>384.99517293613701</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>76.262</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -15955,7 +15922,8 @@
         <v>244.39075838208399</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>67.432000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -15981,7 +15949,8 @@
         <v>179.474769912619</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>58.021000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated the data reference
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Desktop\Final-Research-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gobz\Desktop\Final-Research-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC48B17-1279-46AB-ADD5-DC81EA4090EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD260FD-161D-435E-B589-3C4D0FC3A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{5A61E85F-AC94-470C-89DD-2E206C8F7909}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="RawData" sheetId="1" r:id="rId1"/>
+    <sheet name="Trans1" sheetId="2" r:id="rId2"/>
+    <sheet name="Trans2" sheetId="3" r:id="rId3"/>
+    <sheet name="data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -503,7 +503,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>Trans1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -538,7 +538,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -730,7 +730,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$62</c:f>
+              <c:f>Trans1!$D$2:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -932,7 +932,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$J$1</c:f>
+              <c:f>Trans1!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -967,7 +967,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1159,7 +1159,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$J$2:$J$62</c:f>
+              <c:f>Trans1!$J$2:$J$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1629,7 +1629,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$L$1</c:f>
+              <c:f>Trans1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1664,7 +1664,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -1856,7 +1856,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$L$2:$L$62</c:f>
+              <c:f>Trans1!$L$2:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2295,7 +2295,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>Trans1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2330,7 +2330,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2522,7 +2522,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$62</c:f>
+              <c:f>Trans1!$D$2:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2724,7 +2724,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$L$1</c:f>
+              <c:f>Trans1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2759,7 +2759,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -2951,7 +2951,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$L$2:$L$62</c:f>
+              <c:f>Trans1!$L$2:$L$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3421,7 +3421,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$D$1</c:f>
+              <c:f>Trans1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3456,7 +3456,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3648,7 +3648,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$D$2:$D$62</c:f>
+              <c:f>Trans1!$D$2:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="61"/>
@@ -3850,7 +3850,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$O$1</c:f>
+              <c:f>Trans1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3885,7 +3885,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4077,7 +4077,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$O$2:$O$62</c:f>
+              <c:f>Trans1!$O$2:$O$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4557,7 +4557,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$K$1</c:f>
+              <c:f>Trans1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4692,7 +4692,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$62</c:f>
+              <c:f>Trans1!$B$2:$B$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -4884,7 +4884,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$K$2:$K$62</c:f>
+              <c:f>Trans1!$K$2:$K$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
@@ -13593,7 +13593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750171C9-C24E-4302-9158-F16F3E39D7C7}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -15068,7 +15068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2F29B6-EF92-4EE0-A82D-A0FA9527810B}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>

</xml_diff>